<commit_message>
member upload template updated including missing attributes like gender , age , event id
</commit_message>
<xml_diff>
--- a/member_manage/static/templates/member_upload_template.xlsx
+++ b/member_manage/static/templates/member_upload_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deosanta\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_projects\vymember\member_manage\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8D66AE-9274-4C20-837C-B29DE92380B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8417238C-9743-47D1-88A8-FA0C470857E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -178,69 +178,6 @@
     <t>357 Sunrise Blvd</t>
   </si>
   <si>
-    <t>Maharashtra</t>
-  </si>
-  <si>
-    <t>Karnataka</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>Telangana</t>
-  </si>
-  <si>
-    <t>Tamil Nadu</t>
-  </si>
-  <si>
-    <t>Gujarat</t>
-  </si>
-  <si>
-    <t>Rajasthan</t>
-  </si>
-  <si>
-    <t>West Bengal</t>
-  </si>
-  <si>
-    <t>Punjab</t>
-  </si>
-  <si>
-    <t>Uttar Pradesh</t>
-  </si>
-  <si>
-    <t>Pune</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>New Delhi</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Ahmedabad</t>
-  </si>
-  <si>
-    <t>Jaipur</t>
-  </si>
-  <si>
-    <t>Kolkata</t>
-  </si>
-  <si>
-    <t>Ludhiana</t>
-  </si>
-  <si>
-    <t>Lucknow</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>TechCorp</t>
   </si>
   <si>
@@ -329,6 +266,21 @@
   </si>
   <si>
     <t>2022-10-08</t>
+  </si>
+  <si>
+    <t>event_id</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -387,10 +339,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,15 +657,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -718,32 +688,41 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -755,33 +734,42 @@
       <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2">
+        <v>1682</v>
+      </c>
+      <c r="I2">
+        <v>48723</v>
+      </c>
+      <c r="J2">
+        <v>101</v>
+      </c>
+      <c r="K2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>62</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
         <v>72</v>
       </c>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>93</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -793,33 +781,42 @@
       <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3">
+        <v>1682</v>
+      </c>
+      <c r="I3">
+        <v>48723</v>
+      </c>
+      <c r="J3">
+        <v>101</v>
+      </c>
+      <c r="K3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" t="s">
+      <c r="L3" t="s">
         <v>63</v>
       </c>
-      <c r="H3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3">
+      <c r="M3" s="4">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
-        <v>94</v>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -831,33 +828,42 @@
       <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4">
+        <v>1682</v>
+      </c>
+      <c r="I4">
+        <v>48723</v>
+      </c>
+      <c r="J4">
+        <v>101</v>
+      </c>
+      <c r="K4" t="s">
         <v>54</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>64</v>
       </c>
-      <c r="H4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K4">
+      <c r="M4" s="4">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
-        <v>95</v>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -869,33 +875,42 @@
       <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3">
+        <v>33</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" t="s">
         <v>45</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5">
+        <v>1682</v>
+      </c>
+      <c r="I5">
+        <v>48723</v>
+      </c>
+      <c r="J5">
+        <v>101</v>
+      </c>
+      <c r="K5" t="s">
         <v>55</v>
       </c>
-      <c r="G5" t="s">
+      <c r="L5" t="s">
         <v>65</v>
       </c>
-      <c r="H5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J5" t="s">
-        <v>86</v>
-      </c>
-      <c r="K5">
+      <c r="M5" s="4">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
-        <v>96</v>
+      <c r="N5" s="3">
+        <v>2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -907,33 +922,42 @@
       <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3">
+        <v>34</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
         <v>46</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6">
+        <v>1682</v>
+      </c>
+      <c r="I6">
+        <v>48723</v>
+      </c>
+      <c r="J6">
+        <v>101</v>
+      </c>
+      <c r="K6" t="s">
         <v>56</v>
       </c>
-      <c r="G6" t="s">
+      <c r="L6" t="s">
         <v>66</v>
       </c>
-      <c r="H6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J6" t="s">
-        <v>87</v>
-      </c>
-      <c r="K6">
+      <c r="M6" s="4">
         <v>1</v>
       </c>
-      <c r="L6" t="s">
-        <v>97</v>
+      <c r="N6" s="3">
+        <v>2</v>
+      </c>
+      <c r="O6" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -945,33 +969,42 @@
       <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" t="s">
         <v>47</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7">
+        <v>1682</v>
+      </c>
+      <c r="I7">
+        <v>48723</v>
+      </c>
+      <c r="J7">
+        <v>101</v>
+      </c>
+      <c r="K7" t="s">
         <v>57</v>
       </c>
-      <c r="G7" t="s">
+      <c r="L7" t="s">
         <v>67</v>
       </c>
-      <c r="H7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" t="s">
-        <v>88</v>
-      </c>
-      <c r="K7">
+      <c r="M7" s="4">
         <v>1</v>
       </c>
-      <c r="L7" t="s">
-        <v>98</v>
+      <c r="N7" s="3">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -983,33 +1016,42 @@
       <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s">
         <v>48</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8">
+        <v>1682</v>
+      </c>
+      <c r="I8">
+        <v>48723</v>
+      </c>
+      <c r="J8">
+        <v>101</v>
+      </c>
+      <c r="K8" t="s">
         <v>58</v>
       </c>
-      <c r="G8" t="s">
+      <c r="L8" t="s">
         <v>68</v>
       </c>
-      <c r="H8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" t="s">
-        <v>89</v>
-      </c>
-      <c r="K8">
+      <c r="M8" s="4">
         <v>1</v>
       </c>
-      <c r="L8" t="s">
-        <v>99</v>
+      <c r="N8" s="3">
+        <v>2</v>
+      </c>
+      <c r="O8" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1021,33 +1063,42 @@
       <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9">
+        <v>1682</v>
+      </c>
+      <c r="I9">
+        <v>48723</v>
+      </c>
+      <c r="J9">
+        <v>101</v>
+      </c>
+      <c r="K9" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
+      <c r="L9" t="s">
         <v>69</v>
       </c>
-      <c r="H9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" t="s">
-        <v>90</v>
-      </c>
-      <c r="K9">
+      <c r="M9" s="4">
         <v>2</v>
       </c>
-      <c r="L9" t="s">
-        <v>100</v>
+      <c r="N9" s="3">
+        <v>2</v>
+      </c>
+      <c r="O9" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1059,33 +1110,42 @@
       <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3">
+        <v>25</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" t="s">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10">
+        <v>1682</v>
+      </c>
+      <c r="I10">
+        <v>48723</v>
+      </c>
+      <c r="J10">
+        <v>101</v>
+      </c>
+      <c r="K10" t="s">
         <v>60</v>
       </c>
-      <c r="G10" t="s">
+      <c r="L10" t="s">
         <v>70</v>
       </c>
-      <c r="H10" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10">
+      <c r="M10" s="4">
         <v>2</v>
       </c>
-      <c r="L10" t="s">
-        <v>101</v>
+      <c r="N10" s="3">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1097,29 +1157,38 @@
       <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" t="s">
         <v>51</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11">
+        <v>1682</v>
+      </c>
+      <c r="I11">
+        <v>48723</v>
+      </c>
+      <c r="J11">
+        <v>101</v>
+      </c>
+      <c r="K11" t="s">
         <v>61</v>
       </c>
-      <c r="G11" t="s">
+      <c r="L11" t="s">
         <v>71</v>
       </c>
-      <c r="H11" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" t="s">
-        <v>82</v>
-      </c>
-      <c r="J11" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11">
+      <c r="M11" s="4">
         <v>2</v>
       </c>
-      <c r="L11" t="s">
-        <v>102</v>
+      <c r="N11" s="3">
+        <v>2</v>
+      </c>
+      <c r="O11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>